<commit_message>
Code changes in Prospect.java & ProspectPage.java to implement Create New Prospect.
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/Prospect.xlsx
+++ b/src/test/java/gfl/testData/Prospect.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15420" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
   <oleSize ref="A1"/>
-  <extLst>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>TC0042</t>
   </si>
@@ -106,24 +106,114 @@
     <t>ATEZUBVGSJWU</t>
   </si>
   <si>
-    <t>nmXxtVtADT</t>
-  </si>
-  <si>
     <t>UCN 10119</t>
   </si>
   <si>
-    <t>DkmVj_0304864</t>
-  </si>
-  <si>
-    <t>BYFxN_0304785</t>
+    <t>debqi_0604255</t>
+  </si>
+  <si>
+    <t>nTHBDjtWLP</t>
+  </si>
+  <si>
+    <t>Zaqni_0604404</t>
+  </si>
+  <si>
+    <t>fswwTJMFtO</t>
+  </si>
+  <si>
+    <t>pkXzC_0604977</t>
+  </si>
+  <si>
+    <t>spDCtSsiDh</t>
+  </si>
+  <si>
+    <t>GILJL_0604623</t>
+  </si>
+  <si>
+    <t>poPMyjqCRI</t>
+  </si>
+  <si>
+    <t>jmqHH_0604835</t>
+  </si>
+  <si>
+    <t>IwYrnFdhGf</t>
+  </si>
+  <si>
+    <t>RCfxb_0604328</t>
+  </si>
+  <si>
+    <t>pbAZE_0604317</t>
+  </si>
+  <si>
+    <t>zkErYGgcoO</t>
+  </si>
+  <si>
+    <t>SKmSm_0604425</t>
+  </si>
+  <si>
+    <t>QSdCDjFpxR</t>
+  </si>
+  <si>
+    <t>IvtOO_0604688</t>
+  </si>
+  <si>
+    <t>kTJyJeVrjL</t>
+  </si>
+  <si>
+    <t>LuNFD_0604295</t>
+  </si>
+  <si>
+    <t>ikgfAqkTfo</t>
+  </si>
+  <si>
+    <t>QgPWb_0704919</t>
+  </si>
+  <si>
+    <t>dAOcGjqLJR</t>
+  </si>
+  <si>
+    <t>HVxFz_0704737</t>
+  </si>
+  <si>
+    <t>OMkJTcJBfg</t>
+  </si>
+  <si>
+    <t>xSxQw_0704727</t>
+  </si>
+  <si>
+    <t>jOIiTcssJa</t>
+  </si>
+  <si>
+    <t>JtmgF_0704630</t>
+  </si>
+  <si>
+    <t>RwlaAgCBLb</t>
+  </si>
+  <si>
+    <t>fjTIl_0704878</t>
+  </si>
+  <si>
+    <t>NvojoCXEfP</t>
+  </si>
+  <si>
+    <t>kWEze_0704723</t>
+  </si>
+  <si>
+    <t>kkEJGHSthY</t>
+  </si>
+  <si>
+    <t>uLXrR_0704508</t>
+  </si>
+  <si>
+    <t>gCbpvQjCSo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,14 +573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S1048564"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
@@ -501,10 +591,10 @@
     <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
     <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -551,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -559,10 +649,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
@@ -592,7 +682,7 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
         <v>7</v>
@@ -601,7 +691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1048564" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1048564" spans="1:1">
       <c r="A1048564" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Merged and updated code for Prospect Creation workflow
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/Prospect.xlsx
+++ b/src/test/java/gfl/testData/Prospect.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15420" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>TC0042</t>
   </si>
@@ -39,9 +40,6 @@
     <t>BranchBU</t>
   </si>
   <si>
-    <t>GTA HAULING (HIT)</t>
-  </si>
-  <si>
     <t>L1S 1R1</t>
   </si>
   <si>
@@ -99,16 +97,104 @@
     <t>Test</t>
   </si>
   <si>
-    <t>AutoCustUeoLv_0804465</t>
-  </si>
-  <si>
-    <t>JigPzybkuI</t>
+    <t>XFgWvRZZHe</t>
+  </si>
+  <si>
+    <t>AutoCustWEFlD_0904119</t>
+  </si>
+  <si>
+    <t>Halifax (HIT)</t>
+  </si>
+  <si>
+    <t>AutoCustzrqRe_0904660</t>
+  </si>
+  <si>
+    <t>iexEkAQRhI</t>
+  </si>
+  <si>
+    <t>AutoCustPXhcB_0904437</t>
+  </si>
+  <si>
+    <t>VjQFbdoCys</t>
+  </si>
+  <si>
+    <t>AutoCustfJmgI_0904155</t>
+  </si>
+  <si>
+    <t>fNaeWiiQEE</t>
+  </si>
+  <si>
+    <t>AutoCustUUaSb_0904978</t>
+  </si>
+  <si>
+    <t>rHHvmyiSsd</t>
+  </si>
+  <si>
+    <t>AutoCustckWib_0904750</t>
+  </si>
+  <si>
+    <t>vrcHZbazPf</t>
+  </si>
+  <si>
+    <t>AutoCustoZocs_0904363</t>
+  </si>
+  <si>
+    <t>nBiBGMrQDN</t>
+  </si>
+  <si>
+    <t>AutoCustlMXPM_0904908</t>
+  </si>
+  <si>
+    <t>rebeKwdbCl</t>
+  </si>
+  <si>
+    <t>AutoCustNymax_0904724</t>
+  </si>
+  <si>
+    <t>BRdvTUxTrD</t>
+  </si>
+  <si>
+    <t>AutoCustcNrZU_0904654</t>
+  </si>
+  <si>
+    <t>xCvDTdegUL</t>
+  </si>
+  <si>
+    <t>AutoCustCeQTv_0904575</t>
+  </si>
+  <si>
+    <t>oaTjaTeGKd</t>
+  </si>
+  <si>
+    <t>AutoCustjccQM_0904614</t>
+  </si>
+  <si>
+    <t>zLZMOaktMM</t>
+  </si>
+  <si>
+    <t>AutoCustAeZbc_0904936</t>
+  </si>
+  <si>
+    <t>MRJzRbAJdn</t>
+  </si>
+  <si>
+    <t>AutoCustggwnM_0904546</t>
+  </si>
+  <si>
+    <t>YmctqZnLaO</t>
+  </si>
+  <si>
+    <t>AutoCustALZpy_0904915</t>
+  </si>
+  <si>
+    <t>QZRuvceAQg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -462,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,26 +558,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O1048564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -511,163 +597,169 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="F2" s="2">
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2">
         <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2">
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="L3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N3">
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2">
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4">
         <v>3</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="1048564" spans="1:1">

</xml_diff>

<commit_message>
Updated code to fetch the signature dyanmically.
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/Prospect.xlsx
+++ b/src/test/java/gfl/testData/Prospect.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
   <si>
     <t>TC0042</t>
   </si>
@@ -200,6 +200,216 @@
   </si>
   <si>
     <t>AutoCustqybiE_0904774</t>
+  </si>
+  <si>
+    <t>AutoCustSBuQZ_1004779</t>
+  </si>
+  <si>
+    <t>XxImQeKaQo</t>
+  </si>
+  <si>
+    <t>AutoCustvfJcG_1004663</t>
+  </si>
+  <si>
+    <t>DZvGiTHoiM</t>
+  </si>
+  <si>
+    <t>AutoCustimXtD_1004556</t>
+  </si>
+  <si>
+    <t>UxwCvPlpoY</t>
+  </si>
+  <si>
+    <t>AutoCustlQtgo_1004223</t>
+  </si>
+  <si>
+    <t>IGweSnPrgw</t>
+  </si>
+  <si>
+    <t>AutoCustgxqWf_1004222</t>
+  </si>
+  <si>
+    <t>UKVGBikpSd</t>
+  </si>
+  <si>
+    <t>AutoCusthpBJt_1004445</t>
+  </si>
+  <si>
+    <t>bFDVsKsKtf</t>
+  </si>
+  <si>
+    <t>AutoCustggbYR_1004348</t>
+  </si>
+  <si>
+    <t>dALjMnXStD</t>
+  </si>
+  <si>
+    <t>AutoCustjKWog_1004395</t>
+  </si>
+  <si>
+    <t>KrEVmRzvCQ</t>
+  </si>
+  <si>
+    <t>AutoCustJoYMd_1004824</t>
+  </si>
+  <si>
+    <t>Ciozqfjfik</t>
+  </si>
+  <si>
+    <t>AutoCustvrTQo_1004988</t>
+  </si>
+  <si>
+    <t>rIKLqxHSmD</t>
+  </si>
+  <si>
+    <t>AutoCustTFaCd_1004988</t>
+  </si>
+  <si>
+    <t>xGBxaqWLHA</t>
+  </si>
+  <si>
+    <t>AutoCustAissz_1004187</t>
+  </si>
+  <si>
+    <t>UvIznAvynP</t>
+  </si>
+  <si>
+    <t>AutoCustwogch_1004443</t>
+  </si>
+  <si>
+    <t>QnVPTgwYcg</t>
+  </si>
+  <si>
+    <t>AutoCusthsGuM_1004238</t>
+  </si>
+  <si>
+    <t>KhWvcwDlrw</t>
+  </si>
+  <si>
+    <t>AutoCustIwIkv_1004482</t>
+  </si>
+  <si>
+    <t>IxsOSjczLj</t>
+  </si>
+  <si>
+    <t>AutoCusttxUzj_1004589</t>
+  </si>
+  <si>
+    <t>VFqBLiCIRt</t>
+  </si>
+  <si>
+    <t>AutoCustypcpX_1004825</t>
+  </si>
+  <si>
+    <t>cEUJbzDHka</t>
+  </si>
+  <si>
+    <t>AutoCustoSJQr_1004477</t>
+  </si>
+  <si>
+    <t>sjdCDRJoFc</t>
+  </si>
+  <si>
+    <t>AutoCustUORcf_1004190</t>
+  </si>
+  <si>
+    <t>hBNefmxvyU</t>
+  </si>
+  <si>
+    <t>AutoCustyBDqo_1004913</t>
+  </si>
+  <si>
+    <t>dqsiOKrZpD</t>
+  </si>
+  <si>
+    <t>AutoCustcsgxP_1004165</t>
+  </si>
+  <si>
+    <t>hTCyCBItOh</t>
+  </si>
+  <si>
+    <t>AutoCustiArPK_1004894</t>
+  </si>
+  <si>
+    <t>DGZLSifVtZ</t>
+  </si>
+  <si>
+    <t>AutoCustNfxBC_1304139</t>
+  </si>
+  <si>
+    <t>cbOZcvMCcj</t>
+  </si>
+  <si>
+    <t>AutoCustbvxgX_1304954</t>
+  </si>
+  <si>
+    <t>AutoCustLPOVj_1304906</t>
+  </si>
+  <si>
+    <t>sHFXJDVVxt</t>
+  </si>
+  <si>
+    <t>AutoCustGVjZL_1304481</t>
+  </si>
+  <si>
+    <t>oXRbUfRrhY</t>
+  </si>
+  <si>
+    <t>AutoCustjsavm_1304472</t>
+  </si>
+  <si>
+    <t>rXxwfCuLQy</t>
+  </si>
+  <si>
+    <t>AutoCustgEYUd_1304926</t>
+  </si>
+  <si>
+    <t>dlIvOlQJXe</t>
+  </si>
+  <si>
+    <t>AutoCustDecaM_1304937</t>
+  </si>
+  <si>
+    <t>ZRVQmLxRpI</t>
+  </si>
+  <si>
+    <t>AutoCustHDaaK_1304385</t>
+  </si>
+  <si>
+    <t>exxNLXGCFA</t>
+  </si>
+  <si>
+    <t>AutoCustSlNDG_1304860</t>
+  </si>
+  <si>
+    <t>udVikJmSeL</t>
+  </si>
+  <si>
+    <t>AutoCustOYwyg_1304287</t>
+  </si>
+  <si>
+    <t>vScLkwuZIy</t>
+  </si>
+  <si>
+    <t>AutoCustKhpDv_1304485</t>
+  </si>
+  <si>
+    <t>jiNDDhvFGZ</t>
+  </si>
+  <si>
+    <t>AutoCustZwWfk_1304288</t>
+  </si>
+  <si>
+    <t>dJTiprpGbD</t>
+  </si>
+  <si>
+    <t>AutoCustbIfYs_1304584</t>
+  </si>
+  <si>
+    <t>nTJvJrcVpn</t>
+  </si>
+  <si>
+    <t>AutoCustQmQaL_1304486</t>
   </si>
 </sst>
 </file>
@@ -647,10 +857,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>27</v>
@@ -694,10 +904,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update code to make script stable.
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/Prospect.xlsx
+++ b/src/test/java/gfl/testData/Prospect.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
   <si>
     <t>TC0042</t>
   </si>
@@ -410,6 +410,54 @@
   </si>
   <si>
     <t>AutoCustQmQaL_1304486</t>
+  </si>
+  <si>
+    <t>AutoCustfCPHf_1304939</t>
+  </si>
+  <si>
+    <t>AutoCustpzWuP_1304430</t>
+  </si>
+  <si>
+    <t>ilCGtBduZP</t>
+  </si>
+  <si>
+    <t>AutoCustNaesq_1304504</t>
+  </si>
+  <si>
+    <t>WRiYTEpmWg</t>
+  </si>
+  <si>
+    <t>AutoCustliosd_1304263</t>
+  </si>
+  <si>
+    <t>PvxKAEQsiu</t>
+  </si>
+  <si>
+    <t>AutoCustDKjWK_1304753</t>
+  </si>
+  <si>
+    <t>AutoCustdtUAS_1304588</t>
+  </si>
+  <si>
+    <t>okUHCZRhFZ</t>
+  </si>
+  <si>
+    <t>AutoCustpmAkV_1404308</t>
+  </si>
+  <si>
+    <t>NjhuAkNcKy</t>
+  </si>
+  <si>
+    <t>AutoCustHQPzh_1404821</t>
+  </si>
+  <si>
+    <t>JIYVRNRiZq</t>
+  </si>
+  <si>
+    <t>AutoCustBkSeA_1404550</t>
+  </si>
+  <si>
+    <t>GPKbpoVpkc</t>
   </si>
 </sst>
 </file>
@@ -857,10 +905,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
did new changes in endtoend flow and added new module
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/Prospect.xlsx
+++ b/src/test/java/gfl/testData/Prospect.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>CustomerName</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Halifax (HIT)</t>
-  </si>
-  <si>
     <t>VehicalName</t>
   </si>
   <si>
@@ -132,21 +129,9 @@
     <t>V_WYZRSSPG</t>
   </si>
   <si>
-    <t>AutoCustFydCq_1604771</t>
-  </si>
-  <si>
-    <t>iCOaYEMXhA</t>
-  </si>
-  <si>
     <t>10165</t>
   </si>
   <si>
-    <t>AutoCustfyDkl_1604952</t>
-  </si>
-  <si>
-    <t>KiDTgZcXwW</t>
-  </si>
-  <si>
     <t>10166</t>
   </si>
   <si>
@@ -160,6 +145,69 @@
   </si>
   <si>
     <t>CAPEX Test Aprover</t>
+  </si>
+  <si>
+    <t>AutoCustJqMGh_2804122</t>
+  </si>
+  <si>
+    <t>AqiWhLTcLT</t>
+  </si>
+  <si>
+    <t>AutoCustRFdnx_2804443</t>
+  </si>
+  <si>
+    <t>xUBzZIPVgX</t>
+  </si>
+  <si>
+    <t>AutoCusteKBnq_2804606</t>
+  </si>
+  <si>
+    <t>SzxxhBTNQM</t>
+  </si>
+  <si>
+    <t>AutoCustaTyRY_2804840</t>
+  </si>
+  <si>
+    <t>AutoCustlLDeQ_2804711</t>
+  </si>
+  <si>
+    <t>ObgXVrKYue</t>
+  </si>
+  <si>
+    <t>AutoCustPDrMr_2804389</t>
+  </si>
+  <si>
+    <t>AutoCustfvLSv_2804759</t>
+  </si>
+  <si>
+    <t>icjsvofGqq</t>
+  </si>
+  <si>
+    <t>AutoCustmxmSm_2804552</t>
+  </si>
+  <si>
+    <t>SWyKFETbUa</t>
+  </si>
+  <si>
+    <t>AutoCustWVLxd_2804232</t>
+  </si>
+  <si>
+    <t>AutoCustEkQKp_2804683</t>
+  </si>
+  <si>
+    <t>lEjajLMzRa</t>
+  </si>
+  <si>
+    <t>AutoCustZKNXH_2804779</t>
+  </si>
+  <si>
+    <t>ZVrXGNKIFC</t>
+  </si>
+  <si>
+    <t>10456</t>
+  </si>
+  <si>
+    <t>AutoCustaagHs_2804611</t>
   </si>
 </sst>
 </file>
@@ -531,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -611,37 +659,37 @@
         <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="Z1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -652,13 +700,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F2" s="2">
         <v>12</v>
@@ -691,28 +739,28 @@
         <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="U2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -723,13 +771,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F3" s="2">
         <v>12</v>
@@ -762,28 +807,28 @@
         <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="U3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>